<commit_message>
xlxs reader funktional (ungetestet)
</commit_message>
<xml_diff>
--- a/DataProcessing/Finanzbericht_Vorlage.xlsx
+++ b/DataProcessing/Finanzbericht_Vorlage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leand\PycharmProjects\kennzahlen-cockpit\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FD93E8D-2239-4D98-B3E4-40AE8F95AFC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C06501-8F56-4F13-9211-2C193DA38258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="23328" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5496" yWindow="420" windowWidth="23328" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bilanz" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Flüssige Mittel</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Verbindlichkeiten L+L</t>
   </si>
   <si>
-    <t>Bankshuld</t>
-  </si>
-  <si>
     <t>Langfristiges Fremdkapital</t>
   </si>
   <si>
@@ -173,9 +170,6 @@
     <t>Betriebsertrag</t>
   </si>
   <si>
-    <t>Verluste aus Forderungen</t>
-  </si>
-  <si>
     <t>Ertrag Immobilien</t>
   </si>
   <si>
@@ -189,9 +183,6 @@
   </si>
   <si>
     <t>Total Ertrag</t>
-  </si>
-  <si>
-    <t>Wertschriften</t>
   </si>
 </sst>
 </file>
@@ -252,7 +243,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -412,24 +403,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="dashed">
-        <color auto="1"/>
-      </left>
-      <right style="dashed">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -449,7 +427,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -754,10 +731,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D49"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J43" sqref="J43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,12 +758,12 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -798,7 +775,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <v>2024</v>
@@ -845,369 +822,342 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="15">
-        <v>44</v>
-      </c>
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="11" t="s">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B11" s="5">
         <v>69</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="12" t="s">
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="7" t="s">
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B13" s="8">
         <v>245</v>
       </c>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
-    </row>
-    <row r="15" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="12" t="s">
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="5">
+        <v>23</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>14</v>
+      <c r="A16" s="13" t="s">
+        <v>15</v>
       </c>
       <c r="B16" s="5">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="5">
+        <v>32</v>
+      </c>
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="5">
-        <v>32</v>
-      </c>
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="10">
-        <f>SUM(B16:B18,B14,B12,B7:B10)</f>
-        <v>576</v>
-      </c>
-      <c r="C19" s="10">
-        <f t="shared" ref="C19:D19" si="0">SUM(C16:C18,C14,C12,C7:C10)</f>
+      <c r="B18" s="10">
+        <f>SUM(B15:B17,B13,B11,B7:B9)</f>
+        <v>532</v>
+      </c>
+      <c r="C18" s="10">
+        <f>SUM(C15:C17,C13,C11,C7:C9)</f>
         <v>0</v>
       </c>
-      <c r="D19" s="10">
-        <f t="shared" si="0"/>
+      <c r="D18" s="10">
+        <f>SUM(D15:D17,D13,D11,D7:D9)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B21" s="5">
         <v>79</v>
       </c>
-      <c r="D22" s="5"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>19</v>
+      <c r="A23" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="B23" s="5">
-        <v>80</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="5">
-        <v>9</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B24" s="5">
+        <v>90</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>22</v>
       </c>
       <c r="B26" s="5">
-        <v>90</v>
-      </c>
-      <c r="C26" s="5"/>
+        <v>150</v>
+      </c>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="5">
+        <v>129</v>
+      </c>
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="13" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B28" s="5">
-        <v>150</v>
+        <v>48</v>
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="5">
-        <v>129</v>
-      </c>
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B30" s="5">
-        <v>48</v>
-      </c>
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="9" t="s">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="10">
-        <f>SUM(B29:B30,B28,B26,B22:B23)</f>
-        <v>576</v>
-      </c>
-      <c r="C31" s="10">
-        <f>SUM(C29:C30,C28,C26,C22:C23)</f>
+      <c r="B29" s="10">
+        <f>SUM(B27:B28,B26,B24,B21:B21)</f>
+        <v>496</v>
+      </c>
+      <c r="C29" s="10">
+        <f>SUM(C27:C28,C26,C24,C21:C21)</f>
         <v>0</v>
       </c>
-      <c r="D31" s="10">
-        <f>SUM(D29:D30,D28,D26,D22:D23)</f>
+      <c r="D29" s="10">
+        <f>SUM(D27:D28,D26,D24,D21:D21)</f>
         <v>0</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B31" s="1">
+        <v>2024</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2021</v>
+      </c>
+      <c r="D31" s="1">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+    </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B33" s="1">
-        <v>2024</v>
-      </c>
-      <c r="C33" s="1">
-        <v>2021</v>
-      </c>
-      <c r="D33" s="1">
-        <v>2022</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="5">
+        <v>79</v>
+      </c>
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="5">
+        <v>43</v>
+      </c>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" s="5">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="D35" s="5"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B36" s="5">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B37" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B38" s="5">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>33</v>
       </c>
       <c r="B39" s="5">
-        <v>1</v>
+        <v>-40</v>
       </c>
       <c r="D39" s="5"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="5">
-        <v>4</v>
-      </c>
-      <c r="D40" s="5"/>
-    </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>34</v>
-      </c>
-      <c r="B41" s="5">
-        <v>-40</v>
-      </c>
-      <c r="D41" s="5"/>
+      <c r="B40" s="10">
+        <f>SUM(B33:B39)</f>
+        <v>131</v>
+      </c>
+      <c r="C40" s="10">
+        <f t="shared" ref="C40:D40" si="0">SUM(C33:C39)</f>
+        <v>0</v>
+      </c>
+      <c r="D40" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="9" t="s">
+      <c r="A42" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>36</v>
       </c>
-      <c r="B42" s="10">
-        <f>SUM(B35:B41)</f>
-        <v>131</v>
-      </c>
-      <c r="C42" s="10">
-        <f t="shared" ref="C42:D42" si="1">SUM(C35:C41)</f>
+      <c r="B43" s="5">
+        <v>234</v>
+      </c>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>37</v>
+      </c>
+      <c r="B44" s="5">
+        <v>45</v>
+      </c>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>38</v>
+      </c>
+      <c r="B45" s="5">
+        <v>23</v>
+      </c>
+      <c r="D45" s="5"/>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B46" s="10">
+        <f>SUM(B43:B45)</f>
+        <v>302</v>
+      </c>
+      <c r="C46" s="10">
+        <f>SUM(C43:C45)</f>
         <v>0</v>
       </c>
-      <c r="D42" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>37</v>
-      </c>
-      <c r="B45" s="5">
-        <v>234</v>
-      </c>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>39</v>
-      </c>
-      <c r="B46" s="5">
-        <v>45</v>
-      </c>
-      <c r="D46" s="5"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>40</v>
-      </c>
-      <c r="B47" s="5">
-        <v>23</v>
-      </c>
-      <c r="D47" s="5"/>
-    </row>
-    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" t="s">
-        <v>38</v>
-      </c>
-      <c r="B48" s="5">
-        <v>-34</v>
-      </c>
-      <c r="D48" s="5"/>
-    </row>
-    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B49" s="10">
-        <f>SUM(B45:B48)</f>
-        <v>268</v>
-      </c>
-      <c r="C49" s="10">
-        <f t="shared" ref="C49:D49" si="2">SUM(C45:C48)</f>
-        <v>0</v>
-      </c>
-      <c r="D49" s="10">
-        <f t="shared" si="2"/>
+      <c r="D46" s="10">
+        <f>SUM(D43:D45)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
xlxs_reader quick fix (reingewinn removed from excel)
</commit_message>
<xml_diff>
--- a/DataProcessing/Finanzbericht_Vorlage.xlsx
+++ b/DataProcessing/Finanzbericht_Vorlage.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leand\PycharmProjects\kennzahlen-cockpit\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C06501-8F56-4F13-9211-2C193DA38258}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1D9D2-1889-4300-AC17-D3EE6873E39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5496" yWindow="420" windowWidth="23328" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
   <si>
     <t>Flüssige Mittel</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t>Finanzaufwand</t>
-  </si>
-  <si>
-    <t>Reingewinn</t>
   </si>
   <si>
     <t>Aufwand Immobilien</t>
@@ -731,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A17" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,12 +755,12 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="2">
         <v>3</v>
@@ -1074,9 +1071,9 @@
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="5">
         <v>4</v>
@@ -1084,80 +1081,71 @@
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>33</v>
-      </c>
-      <c r="B39" s="5">
-        <v>-40</v>
-      </c>
-      <c r="D39" s="5"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="9" t="s">
+      <c r="A39" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B39" s="10">
+        <f>SUM(B33:B38)</f>
+        <v>171</v>
+      </c>
+      <c r="C39" s="10">
+        <f>SUM(C33:C38)</f>
+        <v>0</v>
+      </c>
+      <c r="D39" s="10">
+        <f>SUM(D33:D38)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>35</v>
       </c>
-      <c r="B40" s="10">
-        <f>SUM(B33:B39)</f>
-        <v>131</v>
-      </c>
-      <c r="C40" s="10">
-        <f t="shared" ref="C40:D40" si="0">SUM(C33:C39)</f>
-        <v>0</v>
-      </c>
-      <c r="D40" s="10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B42" s="6"/>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
+      <c r="B42" s="5">
+        <v>234</v>
+      </c>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>36</v>
       </c>
       <c r="B43" s="5">
-        <v>234</v>
+        <v>45</v>
       </c>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>37</v>
       </c>
       <c r="B44" s="5">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>38</v>
-      </c>
-      <c r="B45" s="5">
-        <v>23</v>
-      </c>
-      <c r="D45" s="5"/>
-    </row>
-    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A46" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B46" s="10">
-        <f>SUM(B43:B45)</f>
+      <c r="A45" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B45" s="10">
+        <f>SUM(B42:B44)</f>
         <v>302</v>
       </c>
-      <c r="C46" s="10">
-        <f>SUM(C43:C45)</f>
+      <c r="C45" s="10">
+        <f>SUM(C42:C44)</f>
         <v>0</v>
       </c>
-      <c r="D46" s="10">
-        <f>SUM(D43:D45)</f>
+      <c r="D45" s="10">
+        <f>SUM(D42:D44)</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
create main function in xlsx_reader.py and added test files
</commit_message>
<xml_diff>
--- a/DataProcessing/Finanzbericht_Vorlage.xlsx
+++ b/DataProcessing/Finanzbericht_Vorlage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leand\PycharmProjects\kennzahlen-cockpit\DataProcessing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanAtzgerstorfer\PycharmProjects\kennzahlen-cockpit-server\DataProcessing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C1D9D2-1889-4300-AC17-D3EE6873E39F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97204F0C-29EB-4CAA-94E7-6615C5F4BA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5496" yWindow="420" windowWidth="23328" windowHeight="14292" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bilanz" sheetId="1" r:id="rId1"/>
@@ -730,19 +730,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="97" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="44.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.08984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.44140625" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="19" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="14" t="s">
         <v>5</v>
       </c>
@@ -750,7 +750,7 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -758,19 +758,19 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B3" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -784,7 +784,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>0</v>
       </c>
@@ -792,7 +792,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -801,7 +801,7 @@
       </c>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -810,7 +810,7 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -819,7 +819,7 @@
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="11" t="s">
         <v>8</v>
       </c>
@@ -827,7 +827,7 @@
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -837,7 +837,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
@@ -845,7 +845,7 @@
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="7" t="s">
         <v>12</v>
       </c>
@@ -855,7 +855,7 @@
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>13</v>
       </c>
@@ -863,7 +863,7 @@
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -872,7 +872,7 @@
       </c>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
@@ -881,7 +881,7 @@
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="13" t="s">
         <v>16</v>
       </c>
@@ -890,7 +890,7 @@
       </c>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="9" t="s">
         <v>1</v>
       </c>
@@ -907,7 +907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="11" t="s">
         <v>17</v>
       </c>
@@ -915,7 +915,7 @@
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -924,7 +924,7 @@
       </c>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="11" t="s">
         <v>19</v>
       </c>
@@ -932,7 +932,7 @@
       <c r="C22" s="6"/>
       <c r="D22" s="6"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>20</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="13" t="s">
         <v>21</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="12" t="s">
         <v>2</v>
       </c>
@@ -960,7 +960,7 @@
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>22</v>
       </c>
@@ -969,7 +969,7 @@
       </c>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="13" t="s">
         <v>23</v>
       </c>
@@ -978,7 +978,7 @@
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="13" t="s">
         <v>24</v>
       </c>
@@ -987,7 +987,7 @@
       </c>
       <c r="D28" s="5"/>
     </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="9" t="s">
         <v>1</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>2022</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="11" t="s">
         <v>27</v>
       </c>
@@ -1026,7 +1026,7 @@
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -1035,7 +1035,7 @@
       </c>
       <c r="D33" s="5"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>4</v>
       </c>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="D34" s="5"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>30</v>
       </c>
@@ -1053,7 +1053,7 @@
       </c>
       <c r="D35" s="5"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>31</v>
       </c>
@@ -1062,7 +1062,7 @@
       </c>
       <c r="D36" s="5"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1071,7 +1071,7 @@
       </c>
       <c r="D37" s="5"/>
     </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" t="s">
         <v>33</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="D38" s="5"/>
     </row>
-    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="9" t="s">
         <v>34</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="11" t="s">
         <v>28</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="C41" s="6"/>
       <c r="D41" s="6"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="D42" s="5"/>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>36</v>
       </c>
@@ -1123,7 +1123,7 @@
       </c>
       <c r="D43" s="5"/>
     </row>
-    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" t="s">
         <v>37</v>
       </c>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="D44" s="5"/>
     </row>
-    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="9" t="s">
         <v>40</v>
       </c>

</xml_diff>